<commit_message>
dep not working append
</commit_message>
<xml_diff>
--- a/DataBase/KRK_Arrivals.xlsx
+++ b/DataBase/KRK_Arrivals.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3358" uniqueCount="1083">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3498" uniqueCount="1106">
   <si>
     <t>NUMBER</t>
   </si>
@@ -3261,6 +3261,75 @@
   </si>
   <si>
     <t>(SP-LMB)</t>
+  </si>
+  <si>
+    <t>Thursday, Jan 12</t>
+  </si>
+  <si>
+    <t>(9H-VUK)</t>
+  </si>
+  <si>
+    <t>8:31 AM</t>
+  </si>
+  <si>
+    <t>(EI-HEW)</t>
+  </si>
+  <si>
+    <t>9:27 AM</t>
+  </si>
+  <si>
+    <t>RK6249</t>
+  </si>
+  <si>
+    <t>(G-RUKD)</t>
+  </si>
+  <si>
+    <t>9:32 AM</t>
+  </si>
+  <si>
+    <t>0 hours, -23 minutes</t>
+  </si>
+  <si>
+    <t>(EI-HES)</t>
+  </si>
+  <si>
+    <t>9:57 AM</t>
+  </si>
+  <si>
+    <t>10:57 AM</t>
+  </si>
+  <si>
+    <t>(SP-LVA)</t>
+  </si>
+  <si>
+    <t>11:18 AM</t>
+  </si>
+  <si>
+    <t>11:29 AM</t>
+  </si>
+  <si>
+    <t>(SE-RPE)</t>
+  </si>
+  <si>
+    <t>11:33 AM</t>
+  </si>
+  <si>
+    <t>(D-AIEP)</t>
+  </si>
+  <si>
+    <t>0 hours, 29 minutes</t>
+  </si>
+  <si>
+    <t>(LN-DYJ)</t>
+  </si>
+  <si>
+    <t>11:53 AM</t>
+  </si>
+  <si>
+    <t>12:25 PM</t>
+  </si>
+  <si>
+    <t>(G-EZBW)</t>
   </si>
 </sst>
 </file>
@@ -3305,7 +3374,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:M337"/>
+  <dimension ref="A1:M351"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -15752,6 +15821,524 @@
       </c>
       <c r="M337" s="0"/>
     </row>
+    <row r="338">
+      <c r="A338" t="n" s="0">
+        <v>337.0</v>
+      </c>
+      <c r="B338" t="s" s="0">
+        <v>1083</v>
+      </c>
+      <c r="C338" t="s" s="0">
+        <v>440</v>
+      </c>
+      <c r="D338" t="s" s="0">
+        <v>447</v>
+      </c>
+      <c r="E338" t="s" s="0">
+        <v>144</v>
+      </c>
+      <c r="F338" t="s" s="0">
+        <v>145</v>
+      </c>
+      <c r="G338" t="s" s="0">
+        <v>146</v>
+      </c>
+      <c r="H338" t="s" s="0">
+        <v>687</v>
+      </c>
+      <c r="I338" t="s" s="0">
+        <v>688</v>
+      </c>
+      <c r="J338" t="s" s="0">
+        <v>21</v>
+      </c>
+      <c r="K338" s="0"/>
+      <c r="L338" t="s" s="0">
+        <v>236</v>
+      </c>
+      <c r="M338" s="0"/>
+    </row>
+    <row r="339">
+      <c r="A339" t="n" s="0">
+        <v>338.0</v>
+      </c>
+      <c r="B339" t="s" s="0">
+        <v>1083</v>
+      </c>
+      <c r="C339" t="s" s="0">
+        <v>452</v>
+      </c>
+      <c r="D339" t="s" s="0">
+        <v>517</v>
+      </c>
+      <c r="E339" t="s" s="0">
+        <v>262</v>
+      </c>
+      <c r="F339" t="s" s="0">
+        <v>305</v>
+      </c>
+      <c r="G339" t="s" s="0">
+        <v>16</v>
+      </c>
+      <c r="H339" t="s" s="0">
+        <v>61</v>
+      </c>
+      <c r="I339" t="s" s="0">
+        <v>1084</v>
+      </c>
+      <c r="J339" t="s" s="0">
+        <v>1085</v>
+      </c>
+      <c r="K339" s="0"/>
+      <c r="L339" t="s" s="0">
+        <v>475</v>
+      </c>
+      <c r="M339" s="0"/>
+    </row>
+    <row r="340">
+      <c r="A340" t="n" s="0">
+        <v>339.0</v>
+      </c>
+      <c r="B340" t="s" s="0">
+        <v>1083</v>
+      </c>
+      <c r="C340" t="s" s="0">
+        <v>63</v>
+      </c>
+      <c r="D340" t="s" s="0">
+        <v>238</v>
+      </c>
+      <c r="E340" t="s" s="0">
+        <v>87</v>
+      </c>
+      <c r="F340" t="s" s="0">
+        <v>95</v>
+      </c>
+      <c r="G340" t="s" s="0">
+        <v>16</v>
+      </c>
+      <c r="H340" t="s" s="0">
+        <v>61</v>
+      </c>
+      <c r="I340" t="s" s="0">
+        <v>1086</v>
+      </c>
+      <c r="J340" t="s" s="0">
+        <v>1087</v>
+      </c>
+      <c r="K340" s="0"/>
+      <c r="L340" t="s" s="0">
+        <v>539</v>
+      </c>
+      <c r="M340" s="0"/>
+    </row>
+    <row r="341">
+      <c r="A341" t="n" s="0">
+        <v>340.0</v>
+      </c>
+      <c r="B341" t="s" s="0">
+        <v>1083</v>
+      </c>
+      <c r="C341" t="s" s="0">
+        <v>490</v>
+      </c>
+      <c r="D341" t="s" s="0">
+        <v>1088</v>
+      </c>
+      <c r="E341" t="s" s="0">
+        <v>359</v>
+      </c>
+      <c r="F341" t="s" s="0">
+        <v>360</v>
+      </c>
+      <c r="G341" t="s" s="0">
+        <v>16</v>
+      </c>
+      <c r="H341" t="s" s="0">
+        <v>17</v>
+      </c>
+      <c r="I341" t="s" s="0">
+        <v>1089</v>
+      </c>
+      <c r="J341" t="s" s="0">
+        <v>1090</v>
+      </c>
+      <c r="K341" s="0"/>
+      <c r="L341" t="s" s="0">
+        <v>1091</v>
+      </c>
+      <c r="M341" s="0"/>
+    </row>
+    <row r="342">
+      <c r="A342" t="n" s="0">
+        <v>341.0</v>
+      </c>
+      <c r="B342" t="s" s="0">
+        <v>1083</v>
+      </c>
+      <c r="C342" t="s" s="0">
+        <v>747</v>
+      </c>
+      <c r="D342" t="s" s="0">
+        <v>803</v>
+      </c>
+      <c r="E342" t="s" s="0">
+        <v>274</v>
+      </c>
+      <c r="F342" t="s" s="0">
+        <v>275</v>
+      </c>
+      <c r="G342" t="s" s="0">
+        <v>16</v>
+      </c>
+      <c r="H342" t="s" s="0">
+        <v>61</v>
+      </c>
+      <c r="I342" t="s" s="0">
+        <v>1092</v>
+      </c>
+      <c r="J342" t="s" s="0">
+        <v>1093</v>
+      </c>
+      <c r="K342" s="0"/>
+      <c r="L342" t="s" s="0">
+        <v>539</v>
+      </c>
+      <c r="M342" s="0"/>
+    </row>
+    <row r="343">
+      <c r="A343" t="n" s="0">
+        <v>342.0</v>
+      </c>
+      <c r="B343" t="s" s="0">
+        <v>1083</v>
+      </c>
+      <c r="C343" t="s" s="0">
+        <v>77</v>
+      </c>
+      <c r="D343" t="s" s="0">
+        <v>343</v>
+      </c>
+      <c r="E343" t="s" s="0">
+        <v>175</v>
+      </c>
+      <c r="F343" t="s" s="0">
+        <v>344</v>
+      </c>
+      <c r="G343" t="s" s="0">
+        <v>138</v>
+      </c>
+      <c r="H343" t="s" s="0">
+        <v>61</v>
+      </c>
+      <c r="I343" t="s" s="0">
+        <v>227</v>
+      </c>
+      <c r="J343" t="s" s="0">
+        <v>1094</v>
+      </c>
+      <c r="K343" s="0"/>
+      <c r="L343" t="s" s="0">
+        <v>501</v>
+      </c>
+      <c r="M343" s="0"/>
+    </row>
+    <row r="344">
+      <c r="A344" t="n" s="0">
+        <v>343.0</v>
+      </c>
+      <c r="B344" t="s" s="0">
+        <v>1083</v>
+      </c>
+      <c r="C344" t="s" s="0">
+        <v>142</v>
+      </c>
+      <c r="D344" t="s" s="0">
+        <v>143</v>
+      </c>
+      <c r="E344" t="s" s="0">
+        <v>144</v>
+      </c>
+      <c r="F344" t="s" s="0">
+        <v>145</v>
+      </c>
+      <c r="G344" t="s" s="0">
+        <v>146</v>
+      </c>
+      <c r="H344" t="s" s="0">
+        <v>61</v>
+      </c>
+      <c r="I344" t="s" s="0">
+        <v>1095</v>
+      </c>
+      <c r="J344" t="s" s="0">
+        <v>1096</v>
+      </c>
+      <c r="K344" s="0"/>
+      <c r="L344" t="s" s="0">
+        <v>172</v>
+      </c>
+      <c r="M344" s="0"/>
+    </row>
+    <row r="345">
+      <c r="A345" t="n" s="0">
+        <v>344.0</v>
+      </c>
+      <c r="B345" t="s" s="0">
+        <v>1083</v>
+      </c>
+      <c r="C345" t="s" s="0">
+        <v>516</v>
+      </c>
+      <c r="D345" t="s" s="0">
+        <v>418</v>
+      </c>
+      <c r="E345" t="s" s="0">
+        <v>419</v>
+      </c>
+      <c r="F345" t="s" s="0">
+        <v>420</v>
+      </c>
+      <c r="G345" t="s" s="0">
+        <v>138</v>
+      </c>
+      <c r="H345" t="s" s="0">
+        <v>61</v>
+      </c>
+      <c r="I345" t="s" s="0">
+        <v>222</v>
+      </c>
+      <c r="J345" t="s" s="0">
+        <v>134</v>
+      </c>
+      <c r="K345" s="0"/>
+      <c r="L345" t="s" s="0">
+        <v>236</v>
+      </c>
+      <c r="M345" s="0"/>
+    </row>
+    <row r="346">
+      <c r="A346" t="n" s="0">
+        <v>345.0</v>
+      </c>
+      <c r="B346" t="s" s="0">
+        <v>1083</v>
+      </c>
+      <c r="C346" t="s" s="0">
+        <v>1028</v>
+      </c>
+      <c r="D346" t="s" s="0">
+        <v>523</v>
+      </c>
+      <c r="E346" t="s" s="0">
+        <v>524</v>
+      </c>
+      <c r="F346" t="s" s="0">
+        <v>525</v>
+      </c>
+      <c r="G346" t="s" s="0">
+        <v>106</v>
+      </c>
+      <c r="H346" t="s" s="0">
+        <v>300</v>
+      </c>
+      <c r="I346" t="s" s="0">
+        <v>301</v>
+      </c>
+      <c r="J346" t="s" s="0">
+        <v>1097</v>
+      </c>
+      <c r="K346" s="0"/>
+      <c r="L346" t="s" s="0">
+        <v>191</v>
+      </c>
+      <c r="M346" s="0"/>
+    </row>
+    <row r="347">
+      <c r="A347" t="n" s="0">
+        <v>346.0</v>
+      </c>
+      <c r="B347" t="s" s="0">
+        <v>1083</v>
+      </c>
+      <c r="C347" t="s" s="0">
+        <v>777</v>
+      </c>
+      <c r="D347" t="s" s="0">
+        <v>488</v>
+      </c>
+      <c r="E347" t="s" s="0">
+        <v>419</v>
+      </c>
+      <c r="F347" t="s" s="0">
+        <v>420</v>
+      </c>
+      <c r="G347" t="s" s="0">
+        <v>49</v>
+      </c>
+      <c r="H347" t="s" s="0">
+        <v>17</v>
+      </c>
+      <c r="I347" t="s" s="0">
+        <v>1098</v>
+      </c>
+      <c r="J347" t="s" s="0">
+        <v>1099</v>
+      </c>
+      <c r="K347" s="0"/>
+      <c r="L347" t="s" s="0">
+        <v>206</v>
+      </c>
+      <c r="M347" s="0"/>
+    </row>
+    <row r="348">
+      <c r="A348" t="n" s="0">
+        <v>347.0</v>
+      </c>
+      <c r="B348" t="s" s="0">
+        <v>1083</v>
+      </c>
+      <c r="C348" t="s" s="0">
+        <v>777</v>
+      </c>
+      <c r="D348" t="s" s="0">
+        <v>778</v>
+      </c>
+      <c r="E348" t="s" s="0">
+        <v>65</v>
+      </c>
+      <c r="F348" t="s" s="0">
+        <v>66</v>
+      </c>
+      <c r="G348" t="s" s="0">
+        <v>67</v>
+      </c>
+      <c r="H348" t="s" s="0">
+        <v>107</v>
+      </c>
+      <c r="I348" t="s" s="0">
+        <v>1100</v>
+      </c>
+      <c r="J348" t="s" s="0">
+        <v>963</v>
+      </c>
+      <c r="K348" s="0"/>
+      <c r="L348" t="s" s="0">
+        <v>1101</v>
+      </c>
+      <c r="M348" s="0"/>
+    </row>
+    <row r="349">
+      <c r="A349" t="n" s="0">
+        <v>348.0</v>
+      </c>
+      <c r="B349" t="s" s="0">
+        <v>1083</v>
+      </c>
+      <c r="C349" t="s" s="0">
+        <v>522</v>
+      </c>
+      <c r="D349" t="s" s="0">
+        <v>46</v>
+      </c>
+      <c r="E349" t="s" s="0">
+        <v>47</v>
+      </c>
+      <c r="F349" t="s" s="0">
+        <v>48</v>
+      </c>
+      <c r="G349" t="s" s="0">
+        <v>49</v>
+      </c>
+      <c r="H349" t="s" s="0">
+        <v>17</v>
+      </c>
+      <c r="I349" t="s" s="0">
+        <v>1102</v>
+      </c>
+      <c r="J349" t="s" s="0">
+        <v>1103</v>
+      </c>
+      <c r="K349" s="0"/>
+      <c r="L349" t="s" s="0">
+        <v>172</v>
+      </c>
+      <c r="M349" s="0"/>
+    </row>
+    <row r="350">
+      <c r="A350" t="n" s="0">
+        <v>349.0</v>
+      </c>
+      <c r="B350" t="s" s="0">
+        <v>1083</v>
+      </c>
+      <c r="C350" t="s" s="0">
+        <v>1104</v>
+      </c>
+      <c r="D350" t="s" s="0">
+        <v>408</v>
+      </c>
+      <c r="E350" t="s" s="0">
+        <v>87</v>
+      </c>
+      <c r="F350" t="s" s="0">
+        <v>88</v>
+      </c>
+      <c r="G350" t="s" s="0">
+        <v>16</v>
+      </c>
+      <c r="H350" t="s" s="0">
+        <v>17</v>
+      </c>
+      <c r="I350" t="s" s="0">
+        <v>830</v>
+      </c>
+      <c r="J350" t="s" s="0">
+        <v>783</v>
+      </c>
+      <c r="K350" s="0"/>
+      <c r="L350" t="s" s="0">
+        <v>484</v>
+      </c>
+      <c r="M350" s="0"/>
+    </row>
+    <row r="351">
+      <c r="A351" t="n" s="0">
+        <v>350.0</v>
+      </c>
+      <c r="B351" t="s" s="0">
+        <v>1083</v>
+      </c>
+      <c r="C351" t="s" s="0">
+        <v>548</v>
+      </c>
+      <c r="D351" t="s" s="0">
+        <v>789</v>
+      </c>
+      <c r="E351" t="s" s="0">
+        <v>87</v>
+      </c>
+      <c r="F351" t="s" s="0">
+        <v>638</v>
+      </c>
+      <c r="G351" t="s" s="0">
+        <v>89</v>
+      </c>
+      <c r="H351" t="s" s="0">
+        <v>647</v>
+      </c>
+      <c r="I351" t="s" s="0">
+        <v>1105</v>
+      </c>
+      <c r="J351" t="s" s="0">
+        <v>1031</v>
+      </c>
+      <c r="K351" s="0"/>
+      <c r="L351" t="s" s="0">
+        <v>374</v>
+      </c>
+      <c r="M351" s="0"/>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>